<commit_message>
check-url: make a little edit to the adapt for the task
</commit_message>
<xml_diff>
--- a/check url/links.xlsx
+++ b/check url/links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e9a57eaeee39cc8/Desktop/TOP_projects/check url/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="11_5A1D9E3DE3533E7DC64A0EA402A74203E026AAB0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59396708-DACA-4EB0-A4FE-D1DC4838695D}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="11_5A1D9E3DE3533E7DC64A0EA402A74203E026AAB0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6921D8BC-C1A3-46A9-AAAE-C235B43C60BF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -307,7 +307,7 @@
     <row r="4" spans="1:1" ht="13.2" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{A7BB568E-2663-42CE-81BB-925CD47D3828}"/>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{0C5A280B-7FFD-4B4B-AFF3-B8EAB9D30702}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>